<commit_message>
add comments to treatment parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-treatment.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-treatment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Ponds" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,264 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eg. Formaldehyde</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 6
+Not 6''</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units can be set to (Gal), (ml) or (kg).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1:500</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1.25</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. AB, CD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eg. Formaldehyde</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 6
+Not 6''</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Units can be set to (Gal), (ml) or (kg).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1:500</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1.25</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. AB, CD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Treatment Type</t>
   </si>
@@ -51,15 +307,9 @@
     <t>Duration (hours)</t>
   </si>
   <si>
-    <t>Duration (mins)</t>
-  </si>
-  <si>
     <t>Initials</t>
   </si>
   <si>
-    <t>Pond Level During Treatment (Inches)</t>
-  </si>
-  <si>
     <t>Amount (ml)</t>
   </si>
   <si>
@@ -67,6 +317,9 @@
   </si>
   <si>
     <t>Amount (kg)</t>
+  </si>
+  <si>
+    <t>Water Level During Treatment (Inches)</t>
   </si>
 </sst>
 </file>
@@ -76,7 +329,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +351,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -440,11 +705,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,16 +754,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>1</v>
@@ -507,7 +772,7 @@
         <v>7</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -524,15 +789,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,25 +842,25 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -611,5 +877,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>